<commit_message>
Adding webflux content java8 and salesforce notes
</commit_message>
<xml_diff>
--- a/Others/En France/Les mots.xlsx
+++ b/Others/En France/Les mots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igorromero/NotesInGeneral/Others/En France/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igorgomesromerovilela/Development/NotesInGeneral/Others/En France/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30F36BD-D776-C143-8C70-16FB5DCB5A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F0EBFD-5280-9447-B325-F4A991299022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26880" windowHeight="16800" xr2:uid="{FAB4D674-A391-401D-ACEA-E0147A97A104}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{FAB4D674-A391-401D-ACEA-E0147A97A104}"/>
   </bookViews>
   <sheets>
     <sheet name="MOTS" sheetId="1" r:id="rId1"/>
@@ -189,6 +189,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>connaissez</t>
@@ -4151,6 +4152,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -5001,7 +5003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF14E2DA-1F61-4D3E-BB06-34F5F1D5F3A2}">
   <dimension ref="A1:S95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="142" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="142" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>